<commit_message>
Correcciones en home y note controller
</commit_message>
<xml_diff>
--- a/public/Excel/ejemplo compra 2.xlsx
+++ b/public/Excel/ejemplo compra 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alonso Alavez\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alonso Alavez\Desktop\UAO\isw2\documentos vicsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB41AE7E-4052-4D6D-81BF-295C13DBF3EF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8BCA58-2A99-4CD9-85BF-C730AD148EAA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{68115E53-7DE0-4A83-8128-8BAF0B91DFB8}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$BG$6</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$BG$10</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="105">
   <si>
     <t>Column1</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Column59</t>
   </si>
   <si>
-    <t>09.27.2018</t>
-  </si>
-  <si>
     <t>MX07</t>
   </si>
   <si>
@@ -326,7 +323,40 @@
     <t>867501040441692</t>
   </si>
   <si>
-    <t>867501040412115</t>
+    <t>8952020618373574663</t>
+  </si>
+  <si>
+    <t>SIM TESTING</t>
+  </si>
+  <si>
+    <t>867501041778993</t>
+  </si>
+  <si>
+    <t>SAMSUNG LTE SM-G610M GALAXY J7 PRIME NEG</t>
+  </si>
+  <si>
+    <t>351813093407980</t>
+  </si>
+  <si>
+    <t>08.27.2018</t>
+  </si>
+  <si>
+    <t>APPLE IPHONE 8 PLUS SPACE GRAY 64GB-LAE</t>
+  </si>
+  <si>
+    <t>359499088075073</t>
+  </si>
+  <si>
+    <t>ZTE LTE BLADE V8 SE DORADO</t>
+  </si>
+  <si>
+    <t>863243032071559</t>
+  </si>
+  <si>
+    <t>SIM TESTING 2</t>
+  </si>
+  <si>
+    <t>8952020618373574664</t>
   </si>
 </sst>
 </file>
@@ -592,8 +622,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF6C83E1-F6DB-42BA-BD3A-E2AD0432ACE0}" name="_0199544039" displayName="_0199544039" ref="A1:BG6" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:BG6" xr:uid="{C38CD604-BB23-43C5-AEA6-B1AF14305ECC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF6C83E1-F6DB-42BA-BD3A-E2AD0432ACE0}" name="_0199544039" displayName="_0199544039" ref="A1:BG10" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:BG10" xr:uid="{C38CD604-BB23-43C5-AEA6-B1AF14305ECC}"/>
   <tableColumns count="59">
     <tableColumn id="1" xr3:uid="{D6C86C9A-FFF3-4CC1-BC93-CB743C64095B}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="44"/>
     <tableColumn id="2" xr3:uid="{25BC19D5-0D74-4341-B4AC-ADEEE86325BC}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="43"/>
@@ -956,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A3C7B5-97FC-4A9B-87E1-0F699DE488E9}">
-  <dimension ref="A1:BG6"/>
+  <dimension ref="A1:BG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -991,7 +1021,7 @@
     <col min="31" max="34" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="35.77734375" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="39" max="52" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="11.77734375" bestFit="1" customWidth="1"/>
@@ -1183,91 +1213,91 @@
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="D2" s="2">
         <v>0.54217592592592589</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="G2">
         <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I2">
         <v>11</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="O2">
         <v>12</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q2">
         <v>58439</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="T2">
         <v>10170523</v>
       </c>
       <c r="U2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="AB2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD2">
         <v>594468096</v>
@@ -1276,61 +1306,61 @@
         <v>10</v>
       </c>
       <c r="AF2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG2" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="AH2">
         <v>70013043</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AJ2">
         <v>1</v>
       </c>
       <c r="AK2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM2" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="AN2">
         <v>5152.6000000000004</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AY2">
         <v>5152.6000000000004</v>
@@ -1342,19 +1372,19 @@
         <v>5977.02</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BC2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BD2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="BF2" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="BG2">
         <v>5152.6000000000004</v>
@@ -1362,91 +1392,91 @@
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="D3" s="2">
         <v>0.54217592592592589</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="G3">
         <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I3">
         <v>11</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="O3">
         <v>12</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q3">
         <v>58439</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="T3">
         <v>10170523</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AA3" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="AB3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD3">
         <v>594468096</v>
@@ -1455,61 +1485,61 @@
         <v>20</v>
       </c>
       <c r="AF3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG3" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="AH3">
         <v>70011902</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AJ3">
         <v>4</v>
       </c>
       <c r="AK3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM3" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="AN3">
         <v>6363.48</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AQ3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AU3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AW3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AY3">
         <v>6363.48</v>
@@ -1521,19 +1551,19 @@
         <v>7381.64</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BC3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BD3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE3" s="1" t="s">
+      <c r="BF3" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="BF3" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="BG3">
         <v>1590.87</v>
@@ -1541,91 +1571,91 @@
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="D4" s="2">
         <v>0.54217592592592589</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="G4">
         <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4">
         <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="O4">
         <v>12</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q4">
         <v>58439</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="T4">
         <v>10170523</v>
       </c>
       <c r="U4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AA4" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="AB4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD4">
         <v>594468096</v>
@@ -1634,61 +1664,61 @@
         <v>20</v>
       </c>
       <c r="AF4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG4" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="AH4">
         <v>70011902</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AJ4">
         <v>4</v>
       </c>
       <c r="AK4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM4" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="AN4">
         <v>6363.48</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AQ4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AU4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AV4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AW4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AY4">
         <v>6363.48</v>
@@ -1700,19 +1730,19 @@
         <v>7381.64</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BC4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BD4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE4" s="1" t="s">
+      <c r="BF4" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="BF4" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="BG4">
         <v>1590.87</v>
@@ -1720,91 +1750,91 @@
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2">
         <v>0.54217592592592589</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="G5">
         <v>12</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5">
         <v>11</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="O5">
         <v>12</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q5">
         <v>58439</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="T5">
         <v>10170523</v>
       </c>
       <c r="U5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AA5" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="AB5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD5">
         <v>594468096</v>
@@ -1813,61 +1843,61 @@
         <v>20</v>
       </c>
       <c r="AF5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG5" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="AG5" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="AH5">
         <v>70011902</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AJ5">
         <v>4</v>
       </c>
       <c r="AK5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM5" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="AL5" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM5" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="AN5">
         <v>6363.48</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AR5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AS5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AW5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AY5">
         <v>6363.48</v>
@@ -1879,19 +1909,19 @@
         <v>7381.64</v>
       </c>
       <c r="BB5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BC5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BD5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE5" s="1" t="s">
+      <c r="BF5" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="BF5" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="BG5">
         <v>1590.87</v>
@@ -1899,91 +1929,91 @@
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="D6" s="2">
         <v>0.54217592592592589</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="G6">
         <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6">
         <v>11</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="M6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="O6">
         <v>12</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q6">
         <v>58439</v>
       </c>
       <c r="R6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="T6">
         <v>10170523</v>
       </c>
       <c r="U6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="AA6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AA6" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="AB6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD6">
         <v>594468096</v>
@@ -1992,61 +2022,61 @@
         <v>20</v>
       </c>
       <c r="AF6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG6" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="AG6" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="AH6">
         <v>70011902</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AJ6">
         <v>4</v>
       </c>
       <c r="AK6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM6" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="AL6" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM6" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="AN6">
         <v>6363.48</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AR6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AS6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AU6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AV6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AW6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AY6">
         <v>6363.48</v>
@@ -2058,23 +2088,478 @@
         <v>7381.64</v>
       </c>
       <c r="BB6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BC6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BD6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BE6" s="1" t="s">
+      <c r="BF6" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="BF6" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="BG6">
         <v>1590.87</v>
       </c>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.58384259259259297</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7">
+        <v>11</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7">
+        <v>594468096</v>
+      </c>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7">
+        <v>70011903</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ7">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN7">
+        <v>80</v>
+      </c>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
+      <c r="AR7" s="1"/>
+      <c r="AS7" s="1"/>
+      <c r="AT7" s="1"/>
+      <c r="AU7" s="1"/>
+      <c r="AV7" s="1"/>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="1"/>
+      <c r="BB7" s="1"/>
+      <c r="BC7" s="1"/>
+      <c r="BD7" s="1"/>
+      <c r="BE7" s="1"/>
+      <c r="BF7" s="1"/>
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.62550925925926004</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8">
+        <v>11</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8">
+        <v>594468096</v>
+      </c>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8">
+        <v>70011904</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ8">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN8">
+        <v>4740.5200000000004</v>
+      </c>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="1"/>
+      <c r="BE8" s="1"/>
+      <c r="BF8" s="1"/>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.62550925925926004</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9">
+        <v>13</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9">
+        <v>11</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9">
+        <v>594468097</v>
+      </c>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9">
+        <v>70012064</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ9">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AM9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN9" s="1">
+        <v>15528.46</v>
+      </c>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="1"/>
+      <c r="BE9" s="1"/>
+      <c r="BF9" s="1"/>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.667175925925927</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <v>13</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10">
+        <v>11</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10">
+        <v>594468097</v>
+      </c>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10">
+        <v>70011364</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ10">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN10" s="1">
+        <v>2174.3200000000002</v>
+      </c>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="1"/>
+      <c r="BF10" s="1"/>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.58384259259259297</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11">
+        <v>12</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11">
+        <v>11</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11">
+        <v>594468096</v>
+      </c>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11">
+        <v>70011903</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ11">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN11">
+        <v>80</v>
+      </c>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Extract purchase from pdf
</commit_message>
<xml_diff>
--- a/public/Excel/ejemplo compra 2.xlsx
+++ b/public/Excel/ejemplo compra 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alonso Alavez\Desktop\UAO\isw2\documentos vicsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EC8B08-6222-424F-AF89-0109CDCB960A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BD6E0E-8290-45BE-A13C-EF5A9BF503F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{68115E53-7DE0-4A83-8128-8BAF0B91DFB8}"/>
   </bookViews>
@@ -24,11 +24,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -42,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="115">
   <si>
     <t>Column1</t>
   </si>
@@ -378,6 +373,15 @@
   </si>
   <si>
     <t>11.27.2018</t>
+  </si>
+  <si>
+    <t>12.01.2018</t>
+  </si>
+  <si>
+    <t>Equipo de prueba</t>
+  </si>
+  <si>
+    <t>123456789101112</t>
   </si>
 </sst>
 </file>
@@ -410,7 +414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -429,17 +433,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A3C7B5-97FC-4A9B-87E1-0F699DE488E9}">
-  <dimension ref="A1:BG15"/>
+  <dimension ref="A1:BG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL19" sqref="AL19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2511,7 +2529,7 @@
       <c r="BF10" s="1"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="6" t="s">
         <v>98</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2835,6 +2853,65 @@
       </c>
       <c r="AN15">
         <v>4740.5200000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.58384259259259297</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16">
+        <v>12</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16">
+        <v>11</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD16">
+        <v>594468097</v>
+      </c>
+      <c r="AH16">
+        <v>70011904</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ16">
+        <v>1</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN16">
+        <v>5555.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>